<commit_message>
Update with midnight and simplification of the time reading for en and de
</commit_message>
<xml_diff>
--- a/original/de/audio_list.xlsx
+++ b/original/de/audio_list.xlsx
@@ -20,27 +20,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">es ist</t>
   </si>
   <si>
-    <t xml:space="preserve">viertel nach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">halb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">viertel vor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vor</t>
-  </si>
-  <si>
     <t xml:space="preserve">uhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mitternacht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
   </si>
 </sst>
 </file>
@@ -56,6 +146,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,8 +213,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -254,197 +349,325 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:A62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A37"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>1</v>
+      <c r="A8" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>2</v>
+      <c r="A9" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>3</v>
+      <c r="A10" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>4</v>
+      <c r="A11" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>5</v>
+      <c r="A12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>6</v>
+      <c r="A13" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>7</v>
+      <c r="A14" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>8</v>
+      <c r="A15" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>9</v>
+      <c r="A16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <v>10</v>
+      <c r="A17" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>11</v>
+      <c r="A18" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>12</v>
+      <c r="A19" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>13</v>
+      <c r="A20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>14</v>
+      <c r="A21" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>15</v>
+      <c r="A22" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>16</v>
+      <c r="A23" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>17</v>
+      <c r="A24" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>18</v>
+      <c r="A25" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>19</v>
+      <c r="A26" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>20</v>
+      <c r="A27" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>21</v>
+      <c r="A28" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>22</v>
+      <c r="A29" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>23</v>
+      <c r="A30" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>24</v>
+      <c r="A31" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>25</v>
+      <c r="A32" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>26</v>
+      <c r="A33" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>27</v>
+      <c r="A34" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>28</v>
+      <c r="A35" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>29</v>
+      <c r="A36" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>30</v>
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>